<commit_message>
bcd to 7 seg decoder done in logisim
</commit_message>
<xml_diff>
--- a/semestr-1/wde/clock/decoder.xlsx
+++ b/semestr-1/wde/clock/decoder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">7-seg truth table</t>
   </si>
@@ -100,10 +100,22 @@
     <t>B+D+AC+A'D'C'</t>
   </si>
   <si>
-    <t>D+B+A'+C'</t>
+    <t xml:space="preserve">C' + D + A'B' + AB</t>
   </si>
   <si>
     <t>A+B'+D+C</t>
+  </si>
+  <si>
+    <t>D+BA'+B'A'C'+B'AC+C'B</t>
+  </si>
+  <si>
+    <t>A'B+C'A'</t>
+  </si>
+  <si>
+    <t>A'B'+D+CB'+A'C</t>
+  </si>
+  <si>
+    <t>D+A'B+BC'+B'C</t>
   </si>
 </sst>
 </file>
@@ -616,15 +628,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color theme="1"/>
       </left>
@@ -686,6 +689,15 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color theme="1"/>
       </right>
@@ -700,7 +712,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -829,17 +841,17 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="34" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -856,21 +868,12 @@
     <xf fontId="0" fillId="0" borderId="40" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="41" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2111,7 +2114,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00940058-00FB-4DD9-A8A3-00C400BF00C9}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{004B00E9-007B-4E73-8C38-00FA0025002A}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -2128,7 +2131,7 @@
           <xm:sqref>F4:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00DD008D-0085-402D-A14C-000E00940025}">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{002500F0-00A7-48AE-BB23-004E00B100A6}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -2145,7 +2148,7 @@
           <xm:sqref>F4:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{0031003D-00E2-4EF0-B161-00FD00B40027}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{0029008D-0006-4091-843B-009C006C00FD}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -2162,7 +2165,7 @@
           <xm:sqref>B4:E13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{001C00BA-00A5-4252-83AC-003100550070}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00BA0080-004A-4D90-869E-001A00CD0089}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -2179,7 +2182,7 @@
           <xm:sqref>B14:E19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00A000D2-00F5-407A-AADF-009D007F0064}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{009C002E-007C-47F6-BF11-0093007B006F}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -2196,7 +2199,7 @@
           <xm:sqref>B4:E13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{008D0094-00D9-4665-8DC0-004C00E00089}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00220000-00E5-4724-8850-00F5007D002D}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -4341,7 +4344,7 @@
       <c r="H22" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="58" t="s">
+      <c r="I22" s="57" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="57" t="s">
@@ -4430,117 +4433,117 @@
       </c>
     </row>
     <row r="23" s="40" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="60">
-        <v>1</v>
-      </c>
-      <c r="D23" s="61">
-        <v>0</v>
-      </c>
-      <c r="E23" s="62" t="s">
+      <c r="C23" s="59">
+        <v>1</v>
+      </c>
+      <c r="D23" s="60">
+        <v>0</v>
+      </c>
+      <c r="E23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="63">
-        <v>1</v>
-      </c>
-      <c r="H23" s="59" t="s">
+      <c r="F23" s="62">
+        <v>1</v>
+      </c>
+      <c r="H23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="60">
-        <v>1</v>
-      </c>
-      <c r="J23" s="61">
-        <v>1</v>
-      </c>
-      <c r="K23" s="62" t="s">
+      <c r="I23" s="59">
+        <v>1</v>
+      </c>
+      <c r="J23" s="60">
+        <v>1</v>
+      </c>
+      <c r="K23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="L23" s="63">
-        <v>1</v>
-      </c>
-      <c r="N23" s="59" t="s">
+      <c r="L23" s="62">
+        <v>1</v>
+      </c>
+      <c r="N23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="O23" s="60">
-        <v>1</v>
-      </c>
-      <c r="P23" s="61">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="62" t="s">
+      <c r="O23" s="59">
+        <v>1</v>
+      </c>
+      <c r="P23" s="60">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="R23" s="63">
-        <v>1</v>
-      </c>
-      <c r="T23" s="59" t="s">
+      <c r="R23" s="62">
+        <v>1</v>
+      </c>
+      <c r="T23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="U23" s="60">
-        <v>1</v>
-      </c>
-      <c r="V23" s="61">
-        <v>0</v>
-      </c>
-      <c r="W23" s="62" t="s">
+      <c r="U23" s="59">
+        <v>1</v>
+      </c>
+      <c r="V23" s="60">
+        <v>0</v>
+      </c>
+      <c r="W23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="X23" s="63">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="59" t="s">
+      <c r="X23" s="62">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AA23" s="60">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="62">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="62" t="s">
+      <c r="AA23" s="59">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="61">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="AD23" s="63">
-        <v>1</v>
-      </c>
-      <c r="AF23" s="59" t="s">
+      <c r="AD23" s="62">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AG23" s="60">
-        <v>1</v>
-      </c>
-      <c r="AH23" s="62">
-        <v>1</v>
-      </c>
-      <c r="AI23" s="62" t="s">
+      <c r="AG23" s="59">
+        <v>1</v>
+      </c>
+      <c r="AH23" s="61">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="AJ23" s="63">
-        <v>1</v>
-      </c>
-      <c r="AL23" s="59" t="s">
+      <c r="AJ23" s="62">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AM23" s="60">
-        <v>0</v>
-      </c>
-      <c r="AN23" s="62">
-        <v>1</v>
-      </c>
-      <c r="AO23" s="62" t="s">
+      <c r="AM23" s="59">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="61">
+        <v>1</v>
+      </c>
+      <c r="AO23" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="AP23" s="63">
+      <c r="AP23" s="62">
         <v>1</v>
       </c>
     </row>
     <row r="24" s="40" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="63">
         <v>0</v>
       </c>
       <c r="D24" s="40">
@@ -4549,13 +4552,13 @@
       <c r="E24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="65">
-        <v>1</v>
-      </c>
-      <c r="H24" s="59" t="s">
+      <c r="F24" s="64">
+        <v>1</v>
+      </c>
+      <c r="H24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="64">
+      <c r="I24" s="63">
         <v>1</v>
       </c>
       <c r="J24" s="40">
@@ -4564,13 +4567,13 @@
       <c r="K24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="65">
-        <v>1</v>
-      </c>
-      <c r="N24" s="59" t="s">
+      <c r="L24" s="64">
+        <v>1</v>
+      </c>
+      <c r="N24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="64">
+      <c r="O24" s="63">
         <v>1</v>
       </c>
       <c r="P24" s="40">
@@ -4579,13 +4582,13 @@
       <c r="Q24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="R24" s="65">
-        <v>1</v>
-      </c>
-      <c r="T24" s="59" t="s">
+      <c r="R24" s="64">
+        <v>1</v>
+      </c>
+      <c r="T24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="U24" s="64">
+      <c r="U24" s="63">
         <v>0</v>
       </c>
       <c r="V24" s="40">
@@ -4594,13 +4597,13 @@
       <c r="W24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="X24" s="65">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="59" t="s">
+      <c r="X24" s="64">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AA24" s="64">
+      <c r="AA24" s="63">
         <v>0</v>
       </c>
       <c r="AB24" s="40">
@@ -4609,13 +4612,13 @@
       <c r="AC24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AD24" s="65">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="59" t="s">
+      <c r="AD24" s="64">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AG24" s="64">
+      <c r="AG24" s="63">
         <v>0</v>
       </c>
       <c r="AH24" s="40">
@@ -4624,13 +4627,13 @@
       <c r="AI24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AJ24" s="65">
-        <v>1</v>
-      </c>
-      <c r="AL24" s="59" t="s">
+      <c r="AJ24" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AM24" s="64">
+      <c r="AM24" s="63">
         <v>0</v>
       </c>
       <c r="AN24" s="40">
@@ -4639,15 +4642,15 @@
       <c r="AO24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AP24" s="65">
+      <c r="AP24" s="64">
         <v>1</v>
       </c>
     </row>
     <row r="25" s="40" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="63">
         <v>1</v>
       </c>
       <c r="D25" s="40">
@@ -4656,13 +4659,13 @@
       <c r="E25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="65" t="s">
+      <c r="F25" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="59" t="s">
+      <c r="H25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="64">
+      <c r="I25" s="63">
         <v>1</v>
       </c>
       <c r="J25" s="40">
@@ -4671,13 +4674,13 @@
       <c r="K25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="65" t="s">
+      <c r="L25" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="N25" s="59" t="s">
+      <c r="N25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="64">
+      <c r="O25" s="63">
         <v>1</v>
       </c>
       <c r="P25" s="40">
@@ -4686,13 +4689,13 @@
       <c r="Q25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="R25" s="65" t="s">
+      <c r="R25" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="T25" s="59" t="s">
+      <c r="T25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="U25" s="64">
+      <c r="U25" s="63">
         <v>1</v>
       </c>
       <c r="V25" s="40">
@@ -4701,13 +4704,13 @@
       <c r="W25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="X25" s="65" t="s">
+      <c r="X25" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="Z25" s="59" t="s">
+      <c r="Z25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="AA25" s="64">
+      <c r="AA25" s="63">
         <v>0</v>
       </c>
       <c r="AB25" s="40">
@@ -4716,13 +4719,13 @@
       <c r="AC25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AD25" s="65" t="s">
+      <c r="AD25" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="AF25" s="59" t="s">
+      <c r="AF25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="AG25" s="64">
+      <c r="AG25" s="63">
         <v>0</v>
       </c>
       <c r="AH25" s="40">
@@ -4731,13 +4734,13 @@
       <c r="AI25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AJ25" s="65" t="s">
+      <c r="AJ25" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="AL25" s="59" t="s">
+      <c r="AL25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="AM25" s="64">
+      <c r="AM25" s="63">
         <v>1</v>
       </c>
       <c r="AN25" s="40">
@@ -4746,114 +4749,114 @@
       <c r="AO25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AP25" s="65" t="s">
+      <c r="AP25" s="64" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" s="40" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="66">
-        <v>1</v>
-      </c>
-      <c r="D26" s="67">
-        <v>1</v>
-      </c>
-      <c r="E26" s="67" t="s">
+      <c r="C26" s="65">
+        <v>1</v>
+      </c>
+      <c r="D26" s="66">
+        <v>1</v>
+      </c>
+      <c r="E26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="68" t="s">
+      <c r="F26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="59" t="s">
+      <c r="H26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="66">
-        <v>1</v>
-      </c>
-      <c r="J26" s="67">
-        <v>1</v>
-      </c>
-      <c r="K26" s="67" t="s">
+      <c r="I26" s="65">
+        <v>1</v>
+      </c>
+      <c r="J26" s="66">
+        <v>0</v>
+      </c>
+      <c r="K26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="68" t="s">
+      <c r="L26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="N26" s="59" t="s">
+      <c r="N26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="66">
-        <v>0</v>
-      </c>
-      <c r="P26" s="67">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="67" t="s">
+      <c r="O26" s="65">
+        <v>0</v>
+      </c>
+      <c r="P26" s="66">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="R26" s="68" t="s">
+      <c r="R26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="T26" s="59" t="s">
+      <c r="T26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="U26" s="66">
-        <v>1</v>
-      </c>
-      <c r="V26" s="67">
-        <v>1</v>
-      </c>
-      <c r="W26" s="67" t="s">
+      <c r="U26" s="65">
+        <v>1</v>
+      </c>
+      <c r="V26" s="66">
+        <v>1</v>
+      </c>
+      <c r="W26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="X26" s="68" t="s">
+      <c r="X26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="Z26" s="59" t="s">
+      <c r="Z26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="AA26" s="66">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="67">
-        <v>1</v>
-      </c>
-      <c r="AC26" s="67" t="s">
+      <c r="AA26" s="65">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="66">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="AD26" s="68" t="s">
+      <c r="AD26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="AF26" s="59" t="s">
+      <c r="AF26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="AG26" s="66">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="67">
-        <v>1</v>
-      </c>
-      <c r="AI26" s="67" t="s">
+      <c r="AG26" s="65">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="66">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="AJ26" s="68" t="s">
+      <c r="AJ26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="AL26" s="59" t="s">
+      <c r="AL26" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="AM26" s="66">
-        <v>1</v>
-      </c>
-      <c r="AN26" s="67">
-        <v>1</v>
-      </c>
-      <c r="AO26" s="67" t="s">
+      <c r="AM26" s="65">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="66">
+        <v>1</v>
+      </c>
+      <c r="AO26" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="AP26" s="68" t="s">
+      <c r="AP26" s="67" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4862,43 +4865,52 @@
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="70" t="s">
+      <c r="B28" s="68"/>
+      <c r="C28" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="72" t="s">
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
-      <c r="O28" s="74" t="s">
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="O28" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="P28" s="75"/>
-      <c r="Q28" s="75"/>
-      <c r="R28" s="75"/>
-      <c r="U28" s="75"/>
-      <c r="V28" s="75"/>
-      <c r="W28" s="75"/>
-      <c r="X28" s="75"/>
-      <c r="AA28" s="75"/>
-      <c r="AB28" s="75"/>
-      <c r="AC28" s="75"/>
-      <c r="AD28" s="75"/>
-      <c r="AG28" s="75"/>
-      <c r="AH28" s="75"/>
-      <c r="AI28" s="75"/>
-      <c r="AJ28" s="75"/>
-      <c r="AM28" s="75"/>
-      <c r="AN28" s="75"/>
-      <c r="AO28" s="75"/>
-      <c r="AP28" s="75"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
+      <c r="T28" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="U28" s="72"/>
+      <c r="V28" s="72"/>
+      <c r="W28" s="72"/>
+      <c r="X28" s="72"/>
+      <c r="AA28" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB28" s="71"/>
+      <c r="AC28" s="71"/>
+      <c r="AD28" s="71"/>
+      <c r="AG28" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH28" s="71"/>
+      <c r="AI28" s="71"/>
+      <c r="AJ28" s="71"/>
+      <c r="AM28" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN28" s="71"/>
+      <c r="AO28" s="71"/>
+      <c r="AP28" s="71"/>
     </row>
     <row r="29" ht="14.25"/>
     <row r="30" ht="14.25"/>
@@ -22850,7 +22862,7 @@
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="I28:L28"/>
     <mergeCell ref="O28:R28"/>
-    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="T28:X28"/>
     <mergeCell ref="AA28:AD28"/>
     <mergeCell ref="AG28:AJ28"/>
     <mergeCell ref="AM28:AP28"/>
@@ -22863,7 +22875,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00E400AF-00AA-4A74-8A93-006D0091008D}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{002C000B-002F-4EA3-8E07-00A2009C0051}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -22880,7 +22892,92 @@
           <xm:sqref>S4:S13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00EA006E-0049-4385-8BE8-008E00E000FF}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00DF0046-00AC-4970-B989-002B002600FC}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AQ4:AQ13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{008300B9-00F1-4855-8C77-00C200D90027}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AK4:AK13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00E500B4-005F-4293-9E06-005E00AE006E}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AE4:AE13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{008100CA-00D3-4085-9660-00C7005600FB}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>M4:M13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00C90048-0054-47A2-BBE4-000D00F600F9}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>Y4:Y13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{006A0006-009F-43FC-B163-00E6000B002D}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -22897,16 +22994,16 @@
           <xm:sqref>G4:G13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{008900E2-00FA-4B00-BC66-0028000B00C8}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00BF00C6-00B1-4EC3-860A-00FC0064004E}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -22914,16 +23011,16 @@
           <xm:sqref>AQ4:AQ13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{009600CD-00D5-4408-B49E-0040002F00DA}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{005A000E-0028-4C61-BA0E-005D008E0007}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -22931,16 +23028,16 @@
           <xm:sqref>AK4:AK13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00E300BF-00C3-4CE4-9D31-0014003A0066}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{009D0089-000B-4E70-8F1B-00C3001C001E}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -22948,33 +23045,16 @@
           <xm:sqref>AE4:AE13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{005E0013-00A3-4B96-8C1A-0035004D00A3}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{005C007C-0026-4E0E-AEAD-0020006F0016}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>M4:M13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{000F0038-0083-4035-9E6E-00A1003B00AE}">
-            <xm:f>0</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -22982,7 +23062,7 @@
           <xm:sqref>Y4:Y13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00B40051-001C-404D-B59B-004F007800B2}">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{0031000D-0004-482A-8548-003E0079008B}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -22999,7 +23079,7 @@
           <xm:sqref>M4:M13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00CB001E-004D-4D28-92C8-008E00650056}">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00B1004D-00CD-4893-B041-00BE006B0092}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -23016,7 +23096,7 @@
           <xm:sqref>S4:S13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00A50090-0007-49F7-9863-00F40053009B}">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{003200F6-00FA-431C-989B-0071001000E9}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -23033,75 +23113,143 @@
           <xm:sqref>G4:G13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00670087-008C-4CB4-A538-005400310042}">
-            <xm:f>1</xm:f>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00C800D4-00C1-4C3D-B811-004500170069}">
+            <xm:f>0</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF006100"/>
+                <color rgb="FF9C0006"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>AQ4:AQ13</xm:sqref>
+          <xm:sqref>O4:R13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00490006-0073-46F3-BE83-002200D60004}">
-            <xm:f>1</xm:f>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00A90096-0024-4616-9CC9-00170012003A}">
+            <xm:f>0</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF006100"/>
+                <color rgb="FF9C0006"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>AK4:AK13</xm:sqref>
+          <xm:sqref>U4:X13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{007D00CB-00A2-42E2-9ABE-0084009400D8}">
-            <xm:f>1</xm:f>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{000A00D3-00EA-4821-B910-009C0054008F}">
+            <xm:f>0</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF006100"/>
+                <color rgb="FF9C0006"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>AE4:AE13</xm:sqref>
+          <xm:sqref>AG4:AJ13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{000A0092-003E-46C7-BB2E-00AE00C000F5}">
-            <xm:f>1</xm:f>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00A70049-005A-4A3E-93A4-0063004400FA}">
+            <xm:f>0</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF006100"/>
+                <color rgb="FF9C0006"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>Y4:Y13</xm:sqref>
+          <xm:sqref>O14:R19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{0076008B-0008-4772-82BA-008100E6006F}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{008A0077-00F3-4F4F-AEEE-001F008E0071}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I14:L19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{004200C4-0084-4DB2-B801-00EE008E0005}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AA14:AD19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00450005-0038-464B-A925-0064006100D9}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AA4:AD13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00330062-00A5-48C2-A6F5-005C0068007C}">
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>U14:X19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{0079000C-0059-4974-A43F-00E200810033}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -23118,7 +23266,7 @@
           <xm:sqref>C14:F19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00F8001B-00CE-4C20-AB8C-00C800AD00DF}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{005800DB-0059-447F-A90D-009500FB00E7}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -23135,7 +23283,7 @@
           <xm:sqref>C4:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{003700C2-00C3-4641-AF69-00F8009F0063}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00F4004B-0058-4078-B12C-0053004000BA}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -23152,7 +23300,7 @@
           <xm:sqref>I4:L13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{001E0055-00B5-41AF-AF0F-002300700083}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{007F00B6-0012-4F4C-8177-00AF00A700C0}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -23169,7 +23317,7 @@
           <xm:sqref>AM14:AP19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00BE0084-00CD-41DF-855C-004200D6009B}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00D80081-000E-49F1-A09B-000100980093}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -23186,41 +23334,7 @@
           <xm:sqref>AM4:AP13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{007E0092-00AB-4F1B-A7C1-0090004C007A}">
-            <xm:f>0</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I14:L19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00D100C3-0085-4E4E-A8C6-00C3008A004B}">
-            <xm:f>0</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>O4:R13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{003800C3-0071-4B9C-AE43-001C00E700F5}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{002A00E1-004D-4E70-8EB6-007200160009}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -23237,33 +23351,169 @@
           <xm:sqref>AG14:AJ19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{004D00E5-00C9-4BD3-B609-004500050048}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{004C00FA-007B-438C-A34C-00300034008D}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>AG4:AJ13</xm:sqref>
+          <xm:sqref>U4:X13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{006B00AF-007A-4120-8FBF-00E800750016}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{004F00ED-0086-45BB-980E-00CF00A90022}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AA14:AD19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{000500E8-00D8-43FC-8386-005700EE001E}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I4:L13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00350089-006F-4AA8-9281-008E005A00EF}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AG14:AJ19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{0056007B-0035-4234-83AF-003B00B900A3}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AM4:AP13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00EF00E9-00B1-43D1-97BD-00C4004B00DE}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C14:F19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{000700A2-00E8-4A18-891A-00FF004000A0}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C4:F13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00420020-00F0-449F-BCF5-006600300042}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I14:L19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{006E0034-00EC-4C90-BD75-0071005B00A9}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>O4:R13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{004A00F8-00F1-49AA-BCEA-000800F90037}">
+            <xm:f>1</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -23271,50 +23521,16 @@
           <xm:sqref>O14:R19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00EC0024-00BB-40F7-B9F4-00F800720005}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00220051-0089-46DF-819C-00E700F70031}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>U4:X13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00FA0077-0054-42B2-90DB-0091004100A2}">
-            <xm:f>0</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>AA14:AD19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{009C007A-0006-4086-9BD8-002100BC0059}">
-            <xm:f>0</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -23322,16 +23538,16 @@
           <xm:sqref>AA4:AD13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00E10007-007C-44DC-8827-00CD0062007B}">
-            <xm:f>0</xm:f>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{0051009A-002C-46A8-BBE6-000C00B800B9}">
+            <xm:f>1</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF006100"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -23339,7 +23555,7 @@
           <xm:sqref>U14:X19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{005D00D1-0059-4EBB-BA44-003400FF00EE}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{002F0086-0064-43F7-91F1-002F000B0087}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -23356,92 +23572,7 @@
           <xm:sqref>AM14:AP19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00100047-0013-4CB6-9F7A-009C0062009A}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>U14:X19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00EA00F2-00B6-4E6F-8D82-003C006800D0}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>AA4:AD13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{002900D6-008E-433B-A244-008600BF0018}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>O14:R19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00FE00A6-00DF-4E64-94B6-000E000B008D}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>O4:R13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00260008-0091-4556-8A00-004A00420042}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>AA14:AD19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00140053-006E-4EFB-A070-007C004500FA}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00B10052-002F-4680-AAA3-0037008E005D}">
             <xm:f>1</xm:f>
             <x14:dxf>
               <font>
@@ -23457,125 +23588,6 @@
           </x14:cfRule>
           <xm:sqref>AG4:AJ13</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00F50091-00DF-4C68-BE52-000900DA002D}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I14:L19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00C0004C-00E4-4F7E-8BDD-003E009F00EA}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I4:L13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{002200A2-00C1-4F28-9278-00B900970026}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>AG14:AJ19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00B90016-00DF-488C-8469-008B001E0006}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>AM4:AP13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00E90016-00B2-4EFE-BB67-0021001F00B9}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C14:F19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{005F0090-0084-4638-9A2F-003700540051}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C4:F13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00110066-007E-490B-9A93-00DB0049001B}">
-            <xm:f>1</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>U4:X13</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>